<commit_message>
average for sd added
</commit_message>
<xml_diff>
--- a/sd_female_1.xlsx
+++ b/sd_female_1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="19">
   <si>
     <t>MAV , CC</t>
   </si>
@@ -78,6 +78,9 @@
   <si>
     <t>Trace SD</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
@@ -121,7 +124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -324,6 +327,56 @@
         <v>8.677493237617009</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.1267104356470823</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.394840708087148</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.027386657566182946</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5.099255354139058</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.7923208540286591</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4.51010424958433</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.259375965331009</v>
+      </c>
+      <c r="W5" t="n">
+        <v>11.366613164905965</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>3.273445595678131</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.3643718163127525</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>21.187887220686118</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>4.048265039185108</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>5.103645454449996</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.793170618412877</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>11.297946352189092</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -331,7 +384,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -534,6 +587,56 @@
         <v>2.310603576749783</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.24721310380245634</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.116119567459998</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.005259563781964222</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.671025916319976</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.040957435631084456</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1.411935561573671</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.22186560668024377</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3.3470516820028067</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.25329333707696916</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.2364106560868329</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>11.170169837937863</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1.4356784137464385</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2.6724274805177646</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.04094516673840532</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>2.8919217984889407</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -541,7 +644,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -744,6 +847,56 @@
         <v>5.707305260219865</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8382280030529543</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.1057723833851696</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.017714313710554788</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.6127111352173658</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.6035957918432372</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2.101363135251714</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.6526496603509886</v>
+      </c>
+      <c r="W5" t="n">
+        <v>4.48572893811848</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1.4022729412347548</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.1125255342224292</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>9.090860883127664</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>2.597538674056246</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2.6142838971182596</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.6040111984063129</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>5.885256823750043</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -751,7 +904,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -954,6 +1107,56 @@
         <v>4.688164767677102</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3147319037828517</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.348833102459005</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0068649877147410636</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.4192791889348424</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.18767821701167017</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1.7758426106158105</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.2586503642120012</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3.1611374602805156</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.4022031929044953</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.3001925134262595</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>8.791430177359915</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1.6306574741579707</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2.4202334990122707</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.18770187000984653</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>3.1903303989662177</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -961,7 +1164,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1164,6 +1367,56 @@
         <v>12.292906717109489</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5.8428957695909505</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9784217216366143</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.12738078309691164</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5.140334897233011</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2.3204554938983177</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>24.258047309456327</v>
+      </c>
+      <c r="T5" t="n">
+        <v>5.825894925999356</v>
+      </c>
+      <c r="W5" t="n">
+        <v>64.47340462188538</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>23.388939757862477</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.9735869705382898</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>15.688872267264822</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>6.24344812591858</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>5.138687747344227</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>2.328526726689646</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>18.332485206585567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1171,7 +1424,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1374,6 +1627,56 @@
         <v>12.20514463476593</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>8.954585102573107</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.1241725031133079</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.12653368409950969</v>
+      </c>
+      <c r="K5" t="n">
+        <v>6.314277100882539</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2.639481971166968</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>39.52494474970688</v>
+      </c>
+      <c r="T5" t="n">
+        <v>9.333919825213524</v>
+      </c>
+      <c r="W5" t="n">
+        <v>119.48249304444079</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>52.24269293567045</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.1679226396164306</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>20.72043499101095</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>7.958191974252465</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>6.323143486707767</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>2.6441911330793615</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>22.769093805721543</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1381,7 +1684,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1584,6 +1887,56 @@
         <v>5.874710394753278</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8070572946288957</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.2828561683654582</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01846352325138602</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.3119060112729723</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.4689949224555239</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3.5252705165332237</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.7356310083311977</v>
+      </c>
+      <c r="W5" t="n">
+        <v>7.476947342609292</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1.2779591176921283</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.207088467857929</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>13.671330653012317</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>2.6294644824256594</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>3.3179169274251987</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.4693334153369293</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>6.379984643407525</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1591,7 +1944,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1794,6 +2147,56 @@
         <v>6.902576008676439</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6797028189686438</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.2326123313032282</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.018744248498849574</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.7082821575397715</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.6791408519377392</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1.63137475697944</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.5269401994233736</v>
+      </c>
+      <c r="W5" t="n">
+        <v>3.8071183804476436</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1.1573550734131444</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.9734491328158817</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>7.0548865432258525</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>2.0180298964630206</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2.7098886586464896</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.6794617526942971</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>5.086412815715016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1801,7 +2204,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2004,6 +2407,56 @@
         <v>11.484288784634813</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.769300036515664</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9919847365076179</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.08126858592887584</v>
+      </c>
+      <c r="K5" t="n">
+        <v>7.604822517264164</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2.251310638452998</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>19.162054154673754</v>
+      </c>
+      <c r="T5" t="n">
+        <v>4.9276800815263835</v>
+      </c>
+      <c r="W5" t="n">
+        <v>83.20680746805705</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>28.135666193939116</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.2250134072358954</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>30.34793971992549</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>7.2937362146335305</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>7.674026891129357</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>2.2688361437221345</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>29.434704785837738</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2011,7 +2464,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2214,6 +2667,56 @@
         <v>3.8412960775701155</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.23889540291373781</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.878388556178404</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0047328906813413315</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1.8173453119931011</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.06127419014153981</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.9655240461889877</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.204887964145779</v>
+      </c>
+      <c r="W5" t="n">
+        <v>2.0079350431463068</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.22711162055973397</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.359643317916559</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>5.9138308357400815</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1.38059875176416</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1.8176066204849886</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.06123472846283407</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1.8201983760944864</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2221,7 +2724,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2424,6 +2927,56 @@
         <v>5.916079783099616</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.591012410325903</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.3199637673584717</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01981601624778787</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5.220052816803952</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.8555350328466328</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>8.659047857569837</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.5309581150521214</v>
+      </c>
+      <c r="W5" t="n">
+        <v>17.50515034780391</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>6.420032761072121</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.3977051799490414</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>22.847030491812756</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>4.731751000371239</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>5.226515976024809</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.8573342139243323</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>13.51042643778789</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2431,7 +2984,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2634,6 +3187,56 @@
         <v>5.624944444170094</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5652289506247141</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.3459484414905558</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.01211536209952054</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.2465982758491005</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.420245128878707</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1.8963356374223164</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.43159571988265594</v>
+      </c>
+      <c r="W5" t="n">
+        <v>4.309883921967491</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.8072481719421457</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1.0863556158094254</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>10.188057703132296</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1.6040353213140321</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>3.2479779093504177</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.42031037852831155</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>4.270132497962854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>